<commit_message>
start adding to stats
</commit_message>
<xml_diff>
--- a/stats2.xlsx
+++ b/stats2.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="440" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
     <sheet name="Calculator" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Crits" sheetId="6" r:id="rId3"/>
     <sheet name="Old Stats" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -29,8 +29,52 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neel Mehta</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{A9DC0335-736F-8740-8C40-6E265C2BC139}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neel Mehta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">problem: at low levels, each level means an ABSURD amount. it gets less stark as the levels grind onward.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -545,12 +589,6 @@
     <t>Damage</t>
   </si>
   <si>
-    <t>HKO</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
     <t>BaseAttack</t>
   </si>
   <si>
@@ -623,9 +661,6 @@
     <t>TinyLoss</t>
   </si>
   <si>
-    <t>FORMULAE</t>
-  </si>
-  <si>
     <t>Bskl</t>
   </si>
   <si>
@@ -662,19 +697,40 @@
     <t>Form</t>
   </si>
   <si>
-    <t>Gulf</t>
-  </si>
-  <si>
-    <t>Rdiff</t>
-  </si>
-  <si>
-    <t>Rdiff'</t>
-  </si>
-  <si>
     <t>`</t>
   </si>
   <si>
     <t>ExpectedDamage%</t>
+  </si>
+  <si>
+    <t>Lv0</t>
+  </si>
+  <si>
+    <t>FORMULAE - lv20</t>
+  </si>
+  <si>
+    <t>Base Gulf</t>
+  </si>
+  <si>
+    <t>Lv20 Real Gulf</t>
+  </si>
+  <si>
+    <t>Lv0 Real Gulf</t>
+  </si>
+  <si>
+    <t>By Formula (lv20)</t>
+  </si>
+  <si>
+    <t>By Formula (lv0)</t>
+  </si>
+  <si>
+    <t>lv10</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -684,7 +740,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -706,6 +762,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -729,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -739,6 +808,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3066,11 +3136,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F78D61-D830-2644-85BF-423D5462D15F}">
-  <dimension ref="A1:Y32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F78D61-D830-2644-85BF-423D5462D15F}">
+  <dimension ref="A1:AG32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3078,7 +3148,7 @@
     <col min="17" max="17" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>167</v>
       </c>
@@ -3086,16 +3156,16 @@
         <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -3113,21 +3183,21 @@
         <v>170</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>61</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <f>VLOOKUP($A2, Stats!$A:$E, 2)</f>
@@ -3146,186 +3216,212 @@
         <v>120</v>
       </c>
       <c r="I2" s="7">
-        <f>100+(D2-100)*0.4</f>
-        <v>94</v>
+        <f>(D$6+(D2-100)*D$5)*(20+$B2*4)/100</f>
+        <v>22.56</v>
       </c>
       <c r="J2" s="7">
-        <f>60+(E2-100)*0.4</f>
-        <v>54</v>
+        <f t="shared" ref="J2" si="0">(E$6+(E2-100)*E$5)*(20+$B2*4)/100</f>
+        <v>12.96</v>
       </c>
       <c r="K2" s="7">
-        <f>140+(F2-100)*0.8</f>
-        <v>124</v>
+        <f t="shared" ref="K2" si="1">(F$6+(F2-100)*F$5)*(20+$B2*4)/100</f>
+        <v>29.76</v>
       </c>
       <c r="L2" s="7">
-        <f>100+(G2-100)*0.5</f>
-        <v>110</v>
-      </c>
-      <c r="N2">
-        <f>I2-J3</f>
-        <v>50</v>
+        <f t="shared" ref="L2" si="2">(G$6+(G2-100)*G$5)*(20+$B2*4)/100</f>
+        <v>25.92</v>
+      </c>
+      <c r="N2" s="7">
+        <f>MAX(I2-J3,0)</f>
+        <v>8.1599999999999984</v>
       </c>
       <c r="O2" s="4">
         <f>N2/K3</f>
-        <v>0.390625</v>
+        <v>0.2428571428571428</v>
       </c>
       <c r="P2" s="4">
-        <f>MAX((L2-L3)/2+6,0)/100</f>
-        <v>8.5000000000000006E-2</v>
+        <f>MEDIAN((((L2-L3)*100/(20+4*B2))*0.6+6)/100,0,0.5)</f>
+        <v>0.10800000000000004</v>
       </c>
       <c r="Q2" s="8">
         <f>O2+P2*O2</f>
-        <v>0.423828125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0.26908571428571421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f>VLOOKUP($A3, Stats!$A:$E, 2)</f>
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E3">
         <f>VLOOKUP($A3, Stats!$A:$E, 3)</f>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F3">
         <f>VLOOKUP($A3, Stats!$A:$E, 4)</f>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <f>VLOOKUP($A3, Stats!$A:$E, 5)</f>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I4" si="0">100+(D3-100)*0.4</f>
-        <v>112</v>
+        <f>(D$6+(D3-100)*D$5)*(20+$B3*4)/100</f>
+        <v>24</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J4" si="1">60+(E3-100)*0.4</f>
-        <v>44</v>
+        <f t="shared" ref="J3:L3" si="3">(E$6+(E3-100)*E$5)*(20+$B3*4)/100</f>
+        <v>14.4</v>
       </c>
       <c r="K3" s="7">
-        <f t="shared" ref="K3:K4" si="2">140+(F3-100)*0.8</f>
-        <v>128</v>
+        <f t="shared" si="3"/>
+        <v>33.6</v>
       </c>
       <c r="L3" s="7">
-        <f>100+(G3-100)*0.5</f>
-        <v>105</v>
-      </c>
-      <c r="N3">
-        <f>I3-J2</f>
-        <v>58</v>
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="N3" s="7">
+        <f>MAX(I3-J2,0)</f>
+        <v>11.04</v>
       </c>
       <c r="O3" s="4">
         <f>N3/K2</f>
-        <v>0.46774193548387094</v>
-      </c>
-      <c r="P3" s="8">
-        <f>MAX((L3-L2)/2+6,0)/100</f>
-        <v>3.5000000000000003E-2</v>
+        <v>0.37096774193548382</v>
+      </c>
+      <c r="P3" s="4">
+        <f>MEDIAN((((L3-L2)*100/(20+4*B3))*0.6+6)/100,0,0.5)</f>
+        <v>1.1999999999999957E-2</v>
       </c>
       <c r="Q3" s="8">
         <f>O3+P3*O3</f>
-        <v>0.48411290322580641</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0.37541935483870958</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>172</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
-      </c>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5">
+        <v>0.4</v>
+      </c>
+      <c r="E5">
+        <v>0.4</v>
+      </c>
+      <c r="F5">
+        <v>0.8</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>140</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K11" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="K12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12">
-        <f>F12-20*E12</f>
-        <v>40</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>120</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>170</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="U12" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="W12" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ref="D13:D14" si="3">F13-20*E13</f>
-        <v>30</v>
-      </c>
-      <c r="E13">
-        <v>2.5</v>
-      </c>
-      <c r="F13">
-        <v>80</v>
-      </c>
+      <c r="Z12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K13">
         <v>50</v>
       </c>
@@ -3367,24 +3463,39 @@
         <v>50</v>
       </c>
       <c r="X13">
-        <f>100+(W13-100)*0.5</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <v>160</v>
-      </c>
+        <f>100+(W13-100)*0.4</f>
+        <v>80</v>
+      </c>
+      <c r="Z13">
+        <v>50</v>
+      </c>
+      <c r="AA13">
+        <f>R13/5</f>
+        <v>16</v>
+      </c>
+      <c r="AB13">
+        <v>50</v>
+      </c>
+      <c r="AC13">
+        <f>T13/5</f>
+        <v>8</v>
+      </c>
+      <c r="AD13">
+        <v>50</v>
+      </c>
+      <c r="AE13">
+        <f>V13/5</f>
+        <v>20</v>
+      </c>
+      <c r="AF13">
+        <v>50</v>
+      </c>
+      <c r="AG13">
+        <f>X13/5</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K14">
         <v>75</v>
       </c>
@@ -3426,22 +3537,39 @@
         <v>75</v>
       </c>
       <c r="X14">
-        <f t="shared" ref="X14:X17" si="8">100+(W14-100)*0.5</f>
-        <v>87.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15">
-        <f>D12-D13</f>
+        <f t="shared" ref="X14:X17" si="8">100+(W14-100)*0.4</f>
+        <v>90</v>
+      </c>
+      <c r="Z14">
+        <v>75</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" ref="AA14:AG17" si="9">R14/5</f>
+        <v>18</v>
+      </c>
+      <c r="AB14">
+        <v>75</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="F15">
-        <f>F12-F13</f>
-        <v>40</v>
-      </c>
+      <c r="AD14">
+        <v>75</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="AF14">
+        <v>75</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="9"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K15">
         <v>100</v>
       </c>
@@ -3486,19 +3614,36 @@
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>171</v>
-      </c>
-      <c r="D16">
-        <f>D14/D15</f>
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <f>F14/F15</f>
-        <v>4</v>
-      </c>
+      <c r="Z15">
+        <v>100</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="AB15">
+        <v>100</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="AD15">
+        <v>100</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="AF15">
+        <v>100</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K16">
         <v>125</v>
       </c>
@@ -3541,13 +3686,38 @@
       </c>
       <c r="X16">
         <f t="shared" si="8"/>
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>133</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="Z16">
+        <v>125</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="AB16">
+        <v>125</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="AD16">
+        <v>125</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
+      <c r="AF16">
+        <v>125</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K17">
         <v>150</v>
       </c>
@@ -3590,65 +3760,61 @@
       </c>
       <c r="X17">
         <f t="shared" si="8"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C19">
         <v>120</v>
       </c>
-      <c r="D19">
-        <v>135</v>
-      </c>
-      <c r="E19">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C20">
-        <v>80</v>
-      </c>
-      <c r="D20">
-        <v>70</v>
-      </c>
-      <c r="E20">
-        <v>95</v>
-      </c>
+      <c r="Z17">
+        <v>150</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="AB17">
+        <v>150</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="AD17">
+        <v>150</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="AF17">
+        <v>150</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K20" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L20" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C21">
-        <f>C19-C20</f>
-        <v>40</v>
-      </c>
-      <c r="D21">
-        <f>D19-D20</f>
-        <v>65</v>
-      </c>
-      <c r="E21">
-        <f>E19-E20</f>
-        <v>10</v>
-      </c>
+    </row>
+    <row r="21" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K21">
         <v>50</v>
       </c>
@@ -3676,7 +3842,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K22">
         <v>75</v>
       </c>
@@ -3684,27 +3850,27 @@
         <v>120</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" ref="M22:Q25" si="9">$O$17/$L22</f>
+        <f t="shared" ref="M22:M25" si="10">$O$17/$L22</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" ref="N22:N25" si="10">$O$17/$L22*5/4</f>
+        <f t="shared" ref="N22:N25" si="11">$O$17/$L22*5/4</f>
         <v>0.41666666666666663</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" ref="O22:O25" si="11">$O$17/$L22*7/4</f>
+        <f t="shared" ref="O22:O25" si="12">$O$17/$L22*7/4</f>
         <v>0.58333333333333326</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" ref="P22:P25" si="12">$O$17/$L22*3/4</f>
+        <f t="shared" ref="P22:P25" si="13">$O$17/$L22*3/4</f>
         <v>0.25</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" ref="Q22:Q25" si="13">$O$17/$L22*1/4</f>
+        <f t="shared" ref="Q22:Q25" si="14">$O$17/$L22*1/4</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K23">
         <v>100</v>
       </c>
@@ -3712,27 +3878,27 @@
         <v>140</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.3571428571428571</v>
       </c>
       <c r="O23" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="P23" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K24">
         <v>125</v>
       </c>
@@ -3740,27 +3906,27 @@
         <v>160</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.3125</v>
       </c>
       <c r="O24" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.4375</v>
       </c>
       <c r="P24" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.1875</v>
       </c>
       <c r="Q24" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K25">
         <v>150</v>
       </c>
@@ -3768,47 +3934,47 @@
         <v>180</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="O25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.38888888888888884</v>
       </c>
       <c r="P25" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K27" t="s">
+        <v>201</v>
+      </c>
+      <c r="L27" t="s">
         <v>204</v>
       </c>
-      <c r="L27" t="s">
-        <v>207</v>
-      </c>
       <c r="M27" t="s">
+        <v>202</v>
+      </c>
+      <c r="N27" t="s">
         <v>205</v>
       </c>
-      <c r="N27" t="s">
-        <v>208</v>
-      </c>
       <c r="O27" t="s">
+        <v>203</v>
+      </c>
+      <c r="P27" t="s">
         <v>206</v>
       </c>
-      <c r="P27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K28">
         <v>100</v>
       </c>
@@ -3829,7 +3995,7 @@
         <v>12.25</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K29">
         <v>100</v>
       </c>
@@ -3846,11 +4012,11 @@
         <v>0.09</v>
       </c>
       <c r="P29" s="6">
-        <f t="shared" ref="P29:P31" si="14">MAX((L29-N29)/8+6,0)</f>
+        <f t="shared" ref="P29:P31" si="15">MAX((L29-N29)/8+6,0)</f>
         <v>9.125</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K30">
         <v>100</v>
       </c>
@@ -3867,11 +4033,11 @@
         <v>0.06</v>
       </c>
       <c r="P30" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K31">
         <v>100</v>
       </c>
@@ -3888,11 +4054,11 @@
         <v>0.03</v>
       </c>
       <c r="P31" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.875</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="11:33" x14ac:dyDescent="0.2">
       <c r="K32">
         <v>100</v>
       </c>
@@ -3916,15 +4082,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814FD987-7A47-2D49-9394-F1DF7A51FC34}">
-  <dimension ref="B1:L31"/>
+  <dimension ref="B1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27:K30"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3935,23 +4102,24 @@
     <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="43.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
@@ -3999,7 +4167,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="H4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
@@ -4017,7 +4185,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="H5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -4184,31 +4352,43 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I21" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21" t="s">
         <v>203</v>
       </c>
-      <c r="I21" t="s">
-        <v>210</v>
-      </c>
-      <c r="J21" t="s">
-        <v>206</v>
-      </c>
       <c r="K21" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="L21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="M21" t="s">
+        <v>216</v>
+      </c>
+      <c r="N21" t="s">
+        <v>214</v>
+      </c>
+      <c r="O21" t="s">
+        <v>215</v>
+      </c>
+      <c r="P21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>100</v>
       </c>
@@ -4224,14 +4404,31 @@
       <c r="J22" s="4">
         <v>0.3</v>
       </c>
-      <c r="K22">
-        <v>50</v>
+      <c r="K22" s="9">
+        <v>40</v>
       </c>
       <c r="L22">
+        <f>K22/4</f>
+        <v>10</v>
+      </c>
+      <c r="M22" s="6">
+        <f>(K22-L22)*10/20+L22</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <f>K22*0.6+6</f>
+        <v>30</v>
+      </c>
+      <c r="O22">
+        <f>L22*(20-0)/5*0.6+6</f>
+        <v>30</v>
+      </c>
+      <c r="P22">
+        <f>(M22*80/(20+3*10))*0.6+6</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>150</v>
       </c>
@@ -4247,14 +4444,31 @@
       <c r="J23" s="4">
         <v>0.24</v>
       </c>
-      <c r="K23">
-        <v>37.5</v>
+      <c r="K23" s="9">
+        <v>30</v>
       </c>
       <c r="L23">
+        <f t="shared" ref="L23:L26" si="0">K23/4</f>
+        <v>7.5</v>
+      </c>
+      <c r="M23" s="6">
+        <f t="shared" ref="M23:M26" si="1">(K23-L23)*10/20+L23</f>
         <v>18.75</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N23">
+        <f t="shared" ref="N23:N26" si="2">K23*0.6+6</f>
+        <v>24</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23:P26" si="3">L23*(20-0)/5*0.6+6</f>
+        <v>24</v>
+      </c>
+      <c r="P23">
+        <f t="shared" ref="P23:P26" si="4">(M23*80/(20+3*10))*0.6+6</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>100</v>
       </c>
@@ -4270,14 +4484,31 @@
       <c r="J24" s="4">
         <v>0.18</v>
       </c>
-      <c r="K24">
-        <v>25</v>
+      <c r="K24" s="9">
+        <v>20</v>
       </c>
       <c r="L24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>50</v>
       </c>
@@ -4293,14 +4524,31 @@
       <c r="J25" s="4">
         <v>0.12</v>
       </c>
-      <c r="K25">
-        <v>12.5</v>
+      <c r="K25" s="9">
+        <v>10</v>
       </c>
       <c r="L25">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>150</v>
       </c>
@@ -4316,14 +4564,31 @@
       <c r="J26" s="4">
         <v>0.06</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="9">
         <v>0</v>
       </c>
       <c r="L26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>120</v>
       </c>
@@ -4339,8 +4604,9 @@
       <c r="J27" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>100</v>
       </c>
@@ -4356,8 +4622,9 @@
       <c r="J28" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>50</v>
       </c>
@@ -4373,8 +4640,9 @@
       <c r="J29" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>150</v>
       </c>
@@ -4390,10 +4658,91 @@
       <c r="J30" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>20</v>
+      </c>
+      <c r="P36">
+        <f>100/O36</f>
+        <v>5</v>
+      </c>
+      <c r="Q36">
+        <f>100/(20+N36*4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N37">
+        <v>10</v>
+      </c>
+      <c r="O37">
+        <v>60</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ref="P37:P40" si="5">100/O37</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" ref="Q37:Q40" si="6">100/(20+N37*4)</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N38">
+        <v>20</v>
+      </c>
+      <c r="O38">
+        <v>100</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>24</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="5"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="6"/>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="40" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N40">
+        <v>19</v>
+      </c>
+      <c r="O40">
+        <v>96</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="5"/>
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="6"/>
+        <v>1.0416666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>